<commit_message>
Begin adding classes for Identity and Authentication
</commit_message>
<xml_diff>
--- a/docs/Favesrus_DataModel.xlsx
+++ b/docs/Favesrus_DataModel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\company\Company_Projects\FavitApp\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\company\Company_Projects\Favesrus\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t xml:space="preserve">User </t>
   </si>
@@ -48,9 +47,6 @@
     <t>Category</t>
   </si>
   <si>
-    <t>ModoId</t>
-  </si>
-  <si>
     <t>FavsMap</t>
   </si>
   <si>
@@ -180,22 +176,13 @@
     <t>OccasionId</t>
   </si>
   <si>
-    <t>Phone</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
-    <t>ModoMembershipDate</t>
-  </si>
-  <si>
-    <t>RegCode</t>
-  </si>
-  <si>
-    <t>CardOnFile</t>
-  </si>
-  <si>
     <t>Pic</t>
+  </si>
+  <si>
+    <t>ModoAccountId</t>
   </si>
 </sst>
 </file>
@@ -575,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,21 +574,18 @@
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -613,42 +597,30 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
         <v>51</v>
       </c>
-      <c r="H2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K2" t="s">
-        <v>55</v>
-      </c>
-      <c r="L2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="E3">
         <v>123123</v>
@@ -657,18 +629,18 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4">
         <v>123412</v>
@@ -677,18 +649,18 @@
         <v>41708</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5">
         <v>1231</v>
@@ -697,20 +669,20 @@
         <v>41920</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -718,7 +690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>2</v>
       </c>
@@ -726,7 +698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>3</v>
       </c>
@@ -734,7 +706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2</v>
       </c>
@@ -742,7 +714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>2</v>
       </c>
@@ -750,23 +722,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
         <v>11</v>
       </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -774,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -782,7 +754,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -790,17 +762,17 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -811,7 +783,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -819,7 +791,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -827,7 +799,7 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -835,12 +807,12 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -848,7 +820,7 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -877,27 +849,27 @@
     </row>
     <row r="34" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" t="s">
         <v>16</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" t="s">
         <v>17</v>
-      </c>
-      <c r="D35" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -905,7 +877,7 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36">
         <v>25</v>
@@ -922,7 +894,7 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37">
         <v>50</v>
@@ -939,7 +911,7 @@
         <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38">
         <v>300</v>
@@ -953,18 +925,18 @@
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s">
         <v>21</v>
-      </c>
-      <c r="C41" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -972,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C42" s="8">
         <v>41976</v>
@@ -983,7 +955,7 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C43" s="8">
         <v>41678</v>
@@ -994,7 +966,7 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44" s="8">
         <v>41943</v>
@@ -1002,15 +974,15 @@
     </row>
     <row r="46" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>